<commit_message>
fixed another cut list error
</commit_message>
<xml_diff>
--- a/sketchup/cut list.xlsx
+++ b/sketchup/cut list.xlsx
@@ -4,11 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="120" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="-40" yWindow="120" windowWidth="31340" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$S$1:$AA$13</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -269,8 +273,90 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Colten Nye</author>
+  </authors>
+  <commentList>
+    <comment ref="A5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Colten Nye:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Number of segments for this shape in the entire piece</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Colten Nye:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Numeber of these segs in the entire piece </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Colten Nye:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Number of segments in the piece, OR number of cuts that need made</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -339,7 +425,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,6 +481,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -467,9 +559,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -498,6 +598,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -516,11 +619,8 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="30">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -531,6 +631,10 @@
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -542,6 +646,10 @@
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -881,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -898,74 +1006,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="8" t="s">
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
     </row>
     <row r="2" spans="1:29">
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="9" t="s">
+      <c r="K2" s="8"/>
+      <c r="L2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="S2" s="7" t="s">
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="S2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="7"/>
-      <c r="U2" s="12" t="s">
+      <c r="T2" s="8"/>
+      <c r="U2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
     </row>
     <row r="3" spans="1:29">
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="10" t="s">
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="11" t="s">
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
       <c r="X3" s="12" t="s">
         <v>19</v>
       </c>
@@ -1296,12 +1404,12 @@
         <v>0</v>
       </c>
       <c r="V8" s="1">
+        <f>M8*$D8</f>
+        <v>0</v>
+      </c>
+      <c r="W8" s="1">
         <f>N8*$D8</f>
         <v>54</v>
-      </c>
-      <c r="W8" s="1">
-        <f>O8*$D8</f>
-        <v>0</v>
       </c>
       <c r="X8" s="1">
         <f>O8*$D8</f>
@@ -1558,35 +1666,35 @@
       <c r="O12" s="1">
         <v>6</v>
       </c>
-      <c r="S12" s="5">
+      <c r="S12" s="6">
         <f>J12*$D12</f>
         <v>0</v>
       </c>
-      <c r="T12" s="5">
+      <c r="T12" s="6">
         <f>K12*$D12</f>
         <v>0</v>
       </c>
-      <c r="U12" s="5">
+      <c r="U12" s="6">
         <f>L12*$D12</f>
         <v>0</v>
       </c>
-      <c r="V12" s="5">
+      <c r="V12" s="6">
         <f>M12*$D12</f>
         <v>0</v>
       </c>
-      <c r="W12" s="5">
+      <c r="W12" s="6">
         <f>N12*$D12</f>
         <v>0</v>
       </c>
-      <c r="X12" s="5">
+      <c r="X12" s="6">
         <f>O12*$D12</f>
         <v>78</v>
       </c>
-      <c r="Y12" s="5">
+      <c r="Y12" s="6">
         <f>P12*$D12</f>
         <v>0</v>
       </c>
-      <c r="Z12" s="5">
+      <c r="Z12" s="6">
         <f>Q12*$D12</f>
         <v>0</v>
       </c>
@@ -1619,11 +1727,11 @@
       </c>
       <c r="V13" s="1">
         <f t="shared" si="4"/>
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="W13" s="1">
         <f t="shared" ref="W13" si="5">SUM(W5:W12)</f>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="X13" s="1">
         <f t="shared" si="4"/>
@@ -1665,11 +1773,11 @@
       </c>
       <c r="V14" s="1">
         <f t="shared" si="6"/>
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="W14" s="1">
         <f t="shared" ref="W14" si="7">W13*W4*0.5</f>
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="X14" s="1">
         <f t="shared" si="6"/>
@@ -1683,15 +1791,15 @@
         <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="AA14" s="6">
+      <c r="AA14" s="7">
         <f>SUM(S14:Z14)</f>
-        <v>381</v>
+        <v>408</v>
       </c>
     </row>
     <row r="15" spans="1:29">
       <c r="AA15" s="1">
         <f>AA14/8</f>
-        <v>47.625</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:29">
@@ -1714,8 +1822,427 @@
     <mergeCell ref="O3:Q3"/>
     <mergeCell ref="L3:N3"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="25">
+      <c r="A1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="25">
+      <c r="A2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="35">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="25">
+      <c r="A5" s="1">
+        <f ca="1">#REF!*$D5</f>
+        <v>48</v>
+      </c>
+      <c r="B5" s="1">
+        <f ca="1">#REF!*$D5</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <f ca="1">#REF!*$D5</f>
+        <v>48</v>
+      </c>
+      <c r="D5" s="1">
+        <f ca="1">#REF!*$D5</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f ca="1">#REF!*$D5</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <f ca="1">#REF!*$D5</f>
+        <v>48</v>
+      </c>
+      <c r="G5" s="1">
+        <f ca="1">#REF!*$D5</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <f ca="1">#REF!*$D5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="25">
+      <c r="A6" s="1">
+        <f ca="1">#REF!*$D6</f>
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <f ca="1">#REF!*$D6</f>
+        <v>24</v>
+      </c>
+      <c r="C6" s="1">
+        <f ca="1">#REF!*$D6</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <f ca="1">#REF!*$D6</f>
+        <v>24</v>
+      </c>
+      <c r="E6" s="1">
+        <f ca="1">#REF!*$D6</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <f ca="1">#REF!*$D6</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <f ca="1">#REF!*$D6</f>
+        <v>24</v>
+      </c>
+      <c r="H6" s="1">
+        <f ca="1">#REF!*$D6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="25">
+      <c r="A7" s="1">
+        <f ca="1">#REF!*$D7</f>
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <f ca="1">#REF!*$D7</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <f ca="1">#REF!*$D7</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <f ca="1">#REF!*$D7</f>
+        <v>18</v>
+      </c>
+      <c r="E7" s="1">
+        <f ca="1">#REF!*$D7</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <f ca="1">#REF!*$D7</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <f ca="1">#REF!*$D7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f ca="1">#REF!*$D7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="25">
+      <c r="A8" s="1">
+        <f ca="1">#REF!*$D8</f>
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <f ca="1">#REF!*$D8</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <f ca="1">#REF!*$D8</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <f ca="1">#REF!*$D8</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <f ca="1">#REF!*$D8</f>
+        <v>54</v>
+      </c>
+      <c r="F8" s="1">
+        <f ca="1">#REF!*$D8</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f ca="1">#REF!*$D8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f ca="1">#REF!*$D8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="25">
+      <c r="A9" s="1">
+        <f ca="1">#REF!*$D9</f>
+        <v>54</v>
+      </c>
+      <c r="B9" s="1">
+        <f ca="1">#REF!*$D9</f>
+        <v>18</v>
+      </c>
+      <c r="C9" s="1">
+        <f ca="1">#REF!*$D9</f>
+        <v>18</v>
+      </c>
+      <c r="D9" s="1">
+        <f ca="1">#REF!*$D9</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <f ca="1">#REF!*$D9</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <f ca="1">#REF!*$D9</f>
+        <v>18</v>
+      </c>
+      <c r="G9" s="1">
+        <f ca="1">#REF!*$D9</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f ca="1">#REF!*$D9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="25">
+      <c r="A10" s="1">
+        <f ca="1">#REF!*$D10</f>
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <f ca="1">#REF!*$D10</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <f ca="1">#REF!*$D10</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <f ca="1">#REF!*$D10</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <f ca="1">#REF!*$D10</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <f ca="1">#REF!*$D10</f>
+        <v>18</v>
+      </c>
+      <c r="G10" s="1">
+        <f ca="1">#REF!*$D10</f>
+        <v>18</v>
+      </c>
+      <c r="H10" s="1">
+        <f ca="1">#REF!*$D10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="25">
+      <c r="A11" s="1">
+        <f ca="1">#REF!*$D11</f>
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <f ca="1">#REF!*$D11</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <f ca="1">#REF!*$D11</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <f ca="1">#REF!*$D11</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <f ca="1">#REF!*$D11</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <f ca="1">#REF!*$D11</f>
+        <v>18</v>
+      </c>
+      <c r="G11" s="1">
+        <f ca="1">#REF!*$D11</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <f ca="1">#REF!*$D11</f>
+        <v>18</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="25">
+      <c r="A12" s="6">
+        <f ca="1">#REF!*$D12</f>
+        <v>0</v>
+      </c>
+      <c r="B12" s="6">
+        <f ca="1">#REF!*$D12</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <f ca="1">#REF!*$D12</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <f ca="1">#REF!*$D12</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <f ca="1">#REF!*$D12</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <f ca="1">#REF!*$D12</f>
+        <v>78</v>
+      </c>
+      <c r="G12" s="6">
+        <f ca="1">#REF!*$D12</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <f ca="1">#REF!*$D12</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="25">
+      <c r="A13" s="1">
+        <f ca="1">SUM(A5:A12)</f>
+        <v>102</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" ref="B13:H13" ca="1" si="0">SUM(B5:B12)</f>
+        <v>42</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="I13" s="1">
+        <f ca="1">SUM(A13:H13)</f>
+        <v>546</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>